<commit_message>
update AES case Aus
</commit_message>
<xml_diff>
--- a/transportation_systems/all_electric_vessels/Prices_modified.xlsx
+++ b/transportation_systems/all_electric_vessels/Prices_modified.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53CCB54-0680-C744-9282-154F3E6B6F39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -79,7 +78,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -356,22 +355,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F169"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="C164" sqref="C164"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" customWidth="1"/>
-    <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -388,7 +387,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>43435.041666666664</v>
       </c>
@@ -408,7 +407,7 @@
         <v>96.8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>43435.083333333336</v>
       </c>
@@ -428,7 +427,7 @@
         <v>80.72</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>43435.125000057873</v>
       </c>
@@ -448,7 +447,7 @@
         <v>69.75</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>43435.16666678241</v>
       </c>
@@ -468,7 +467,7 @@
         <v>76.14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>43435.208333506947</v>
       </c>
@@ -488,7 +487,7 @@
         <v>64.25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>43435.250000231485</v>
       </c>
@@ -508,7 +507,7 @@
         <v>69.87</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>43435.291666956022</v>
       </c>
@@ -528,7 +527,7 @@
         <v>49.49</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>43435.333333680559</v>
       </c>
@@ -548,7 +547,7 @@
         <v>59.45</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>43435.375000405096</v>
       </c>
@@ -568,7 +567,7 @@
         <v>50.92</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>43435.416667129626</v>
       </c>
@@ -588,7 +587,7 @@
         <v>52.77</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>43435.458333854163</v>
       </c>
@@ -608,7 +607,7 @@
         <v>58.28</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>43435.500000578701</v>
       </c>
@@ -628,7 +627,7 @@
         <v>62.47</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>43435.541667303238</v>
       </c>
@@ -648,7 +647,7 @@
         <v>77.400000000000006</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>43435.583334027775</v>
       </c>
@@ -668,7 +667,7 @@
         <v>123.87</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>43435.625000752312</v>
       </c>
@@ -688,7 +687,7 @@
         <v>143.32</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>43435.666667476849</v>
       </c>
@@ -708,7 +707,7 @@
         <v>169.71</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>43435.708334201387</v>
       </c>
@@ -728,7 +727,7 @@
         <v>147.65</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>43435.750000925924</v>
       </c>
@@ -748,7 +747,7 @@
         <v>144.19999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>43435.791667650461</v>
       </c>
@@ -768,7 +767,7 @@
         <v>113.59</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>43435.833334374998</v>
       </c>
@@ -788,7 +787,7 @@
         <v>114.95</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>43435.875001099535</v>
       </c>
@@ -808,7 +807,7 @@
         <v>99.98</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>43435.916667824073</v>
       </c>
@@ -828,7 +827,7 @@
         <v>76.61</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>43435.95833454861</v>
       </c>
@@ -848,7 +847,7 @@
         <v>62.29</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>43436.000001273147</v>
       </c>
@@ -868,7 +867,7 @@
         <v>47.74</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>43436.041667997684</v>
       </c>
@@ -888,7 +887,7 @@
         <v>48.6</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>43436.083334722221</v>
       </c>
@@ -908,7 +907,7 @@
         <v>61.79</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>43436.125001446759</v>
       </c>
@@ -928,7 +927,7 @@
         <v>56.28</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>43436.166666666664</v>
       </c>
@@ -948,7 +947,7 @@
         <v>53.67</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>43436.208333333336</v>
       </c>
@@ -968,7 +967,7 @@
         <v>48.98</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>43436.250001562497</v>
       </c>
@@ -988,7 +987,7 @@
         <v>38.25</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>43436.291668287035</v>
       </c>
@@ -1008,7 +1007,7 @@
         <v>25.73</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>43436.333335011572</v>
       </c>
@@ -1028,7 +1027,7 @@
         <v>47.15</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>43436.375001736109</v>
       </c>
@@ -1048,7 +1047,7 @@
         <v>53.82</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>43436.416668460646</v>
       </c>
@@ -1068,7 +1067,7 @@
         <v>54.67</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>43436.458335185183</v>
       </c>
@@ -1088,7 +1087,7 @@
         <v>121.62</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>43436.500001909721</v>
       </c>
@@ -1108,7 +1107,7 @@
         <v>118.69</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>43436.541668634258</v>
       </c>
@@ -1128,7 +1127,7 @@
         <v>99.86</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>43436.583335358795</v>
       </c>
@@ -1148,7 +1147,7 @@
         <v>156.96</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>43436.625002083332</v>
       </c>
@@ -1168,7 +1167,7 @@
         <v>148.15</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>43436.666668807869</v>
       </c>
@@ -1188,7 +1187,7 @@
         <v>143.08000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>43436.708335532407</v>
       </c>
@@ -1208,7 +1207,7 @@
         <v>120.86</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>43436.750002256944</v>
       </c>
@@ -1228,7 +1227,7 @@
         <v>121.93</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43436.791668981481</v>
       </c>
@@ -1248,7 +1247,7 @@
         <v>123.1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>43436.833335706018</v>
       </c>
@@ -1268,7 +1267,7 @@
         <v>104.03</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>43436.875002430555</v>
       </c>
@@ -1288,7 +1287,7 @@
         <v>84.33</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>43436.916669155093</v>
       </c>
@@ -1308,7 +1307,7 @@
         <v>71.569999999999993</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>43436.95833587963</v>
       </c>
@@ -1328,7 +1327,7 @@
         <v>66.38</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>43437.000002604167</v>
       </c>
@@ -1348,7 +1347,7 @@
         <v>49.64</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>43437.041669328704</v>
       </c>
@@ -1368,7 +1367,7 @@
         <v>35.51</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>43437.083336053242</v>
       </c>
@@ -1388,7 +1387,7 @@
         <v>46.78</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>43437.125002777779</v>
       </c>
@@ -1408,7 +1407,7 @@
         <v>50.14</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>43437.166669502316</v>
       </c>
@@ -1428,7 +1427,7 @@
         <v>41.71</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>43437.208336226853</v>
       </c>
@@ -1448,7 +1447,7 @@
         <v>52.89</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>43437.25000295139</v>
       </c>
@@ -1468,7 +1467,7 @@
         <v>61.38</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>43437.291669675928</v>
       </c>
@@ -1488,7 +1487,7 @@
         <v>79.48</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>43437.333336400465</v>
       </c>
@@ -1508,7 +1507,7 @@
         <v>62.06</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>43437.375003125002</v>
       </c>
@@ -1528,7 +1527,7 @@
         <v>60.2</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>43437.416669849539</v>
       </c>
@@ -1548,7 +1547,7 @@
         <v>61.89</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>43437.458336574076</v>
       </c>
@@ -1568,7 +1567,7 @@
         <v>62.15</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>43437.500003298614</v>
       </c>
@@ -1588,7 +1587,7 @@
         <v>62.17</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>43437.541670023151</v>
       </c>
@@ -1608,7 +1607,7 @@
         <v>60.59</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>43437.583336747688</v>
       </c>
@@ -1628,7 +1627,7 @@
         <v>67.63</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>43437.625003472225</v>
       </c>
@@ -1648,7 +1647,7 @@
         <v>90.11</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>43437.666670196762</v>
       </c>
@@ -1668,7 +1667,7 @@
         <v>99.01</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>43437.7083369213</v>
       </c>
@@ -1688,7 +1687,7 @@
         <v>130.4</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>43437.750003645837</v>
       </c>
@@ -1708,7 +1707,7 @@
         <v>120.38</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>43437.791670370367</v>
       </c>
@@ -1728,7 +1727,7 @@
         <v>134.21</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>43437.833337094904</v>
       </c>
@@ -1748,7 +1747,7 @@
         <v>137.33000000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>43437.875003819441</v>
       </c>
@@ -1768,7 +1767,7 @@
         <v>82.75</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>43437.916670543978</v>
       </c>
@@ -1788,7 +1787,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>43437.958337268516</v>
       </c>
@@ -1808,7 +1807,7 @@
         <v>76.66</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>43438.000003993053</v>
       </c>
@@ -1828,7 +1827,7 @@
         <v>71.91</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>43438.04167071759</v>
       </c>
@@ -1848,7 +1847,7 @@
         <v>65.53</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>43438.083337442127</v>
       </c>
@@ -1868,7 +1867,7 @@
         <v>54.38</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>43438.125004166664</v>
       </c>
@@ -1888,7 +1887,7 @@
         <v>56.72</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>43438.166670891202</v>
       </c>
@@ -1908,7 +1907,7 @@
         <v>55.88</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>43438.208337615739</v>
       </c>
@@ -1928,7 +1927,7 @@
         <v>76.92</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>43438.250004340276</v>
       </c>
@@ -1948,7 +1947,7 @@
         <v>118.68</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>43438.291671064813</v>
       </c>
@@ -1968,7 +1967,7 @@
         <v>91.93</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>43438.33333778935</v>
       </c>
@@ -1988,7 +1987,7 @@
         <v>84.09</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>43438.375004513888</v>
       </c>
@@ -2008,7 +2007,7 @@
         <v>89.17</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>43438.416671238425</v>
       </c>
@@ -2028,7 +2027,7 @@
         <v>96.53</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>43438.458337962962</v>
       </c>
@@ -2048,7 +2047,7 @@
         <v>78.86</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>43438.500004687499</v>
       </c>
@@ -2068,7 +2067,7 @@
         <v>83.27</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>43438.541671412037</v>
       </c>
@@ -2088,7 +2087,7 @@
         <v>99.15</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>43438.583338136574</v>
       </c>
@@ -2108,7 +2107,7 @@
         <v>106.31</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>43438.625004861111</v>
       </c>
@@ -2128,7 +2127,7 @@
         <v>118.47</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>43438.666671585648</v>
       </c>
@@ -2148,7 +2147,7 @@
         <v>89.5</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>43438.708338310185</v>
       </c>
@@ -2168,7 +2167,7 @@
         <v>82.33</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>43438.750005034723</v>
       </c>
@@ -2188,7 +2187,7 @@
         <v>83.7</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>43438.79167175926</v>
       </c>
@@ -2208,7 +2207,7 @@
         <v>95.16</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>43438.833338483797</v>
       </c>
@@ -2228,7 +2227,7 @@
         <v>88.25</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>43438.875005208334</v>
       </c>
@@ -2248,7 +2247,7 @@
         <v>83.4</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>43438.916671932871</v>
       </c>
@@ -2268,7 +2267,7 @@
         <v>64.95</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>43438.958338657409</v>
       </c>
@@ -2288,7 +2287,7 @@
         <v>72.34</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>43439.000005381946</v>
       </c>
@@ -2308,7 +2307,7 @@
         <v>66.02</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>43439.041672106483</v>
       </c>
@@ -2328,7 +2327,7 @@
         <v>57.54</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>43439.08333883102</v>
       </c>
@@ -2348,7 +2347,7 @@
         <v>54.82</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>43439.125005555557</v>
       </c>
@@ -2368,7 +2367,7 @@
         <v>52.34</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>43439.166672280095</v>
       </c>
@@ -2388,7 +2387,7 @@
         <v>56.19</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>43439.208339004632</v>
       </c>
@@ -2408,7 +2407,7 @@
         <v>55.16</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>43439.250005729169</v>
       </c>
@@ -2428,7 +2427,7 @@
         <v>65.59</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>43439.291672453706</v>
       </c>
@@ -2448,7 +2447,7 @@
         <v>80.5</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>43439.333339178243</v>
       </c>
@@ -2468,7 +2467,7 @@
         <v>62.01</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>43439.375005902781</v>
       </c>
@@ -2488,7 +2487,7 @@
         <v>68.17</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>43439.416672627318</v>
       </c>
@@ -2508,7 +2507,7 @@
         <v>89.59</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>43439.458339351855</v>
       </c>
@@ -2528,7 +2527,7 @@
         <v>104.67</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>43439.500006076392</v>
       </c>
@@ -2548,7 +2547,7 @@
         <v>98.12</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>43439.54167280093</v>
       </c>
@@ -2568,7 +2567,7 @@
         <v>91.14</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>43439.583339525459</v>
       </c>
@@ -2588,7 +2587,7 @@
         <v>126.11</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>43439.625006249997</v>
       </c>
@@ -2608,7 +2607,7 @@
         <v>132.78</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>43439.666672974534</v>
       </c>
@@ -2628,7 +2627,7 @@
         <v>92.48</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>43439.708339699071</v>
       </c>
@@ -2648,7 +2647,7 @@
         <v>97.41</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>43439.750006423608</v>
       </c>
@@ -2668,7 +2667,7 @@
         <v>77.739999999999995</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>43439.791673148145</v>
       </c>
@@ -2688,7 +2687,7 @@
         <v>85.9</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>43439.833339872683</v>
       </c>
@@ -2708,7 +2707,7 @@
         <v>80.09</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>43439.87500659722</v>
       </c>
@@ -2728,7 +2727,7 @@
         <v>66.489999999999995</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>43439.916673321757</v>
       </c>
@@ -2748,7 +2747,7 @@
         <v>65.349999999999994</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>43439.958340046294</v>
       </c>
@@ -2768,7 +2767,7 @@
         <v>63.42</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>43440.000006770832</v>
       </c>
@@ -2788,7 +2787,7 @@
         <v>66.8</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>43440.041673495369</v>
       </c>
@@ -2808,7 +2807,7 @@
         <v>54.16</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>43440.083340219906</v>
       </c>
@@ -2828,7 +2827,7 @@
         <v>54.92</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>43440.125006944443</v>
       </c>
@@ -2848,7 +2847,7 @@
         <v>50.35</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>43440.16667366898</v>
       </c>
@@ -2868,7 +2867,7 @@
         <v>51.61</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>43440.208340393518</v>
       </c>
@@ -2888,7 +2887,7 @@
         <v>56.43</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>43440.250007118055</v>
       </c>
@@ -2908,7 +2907,7 @@
         <v>59.62</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>43440.291673842592</v>
       </c>
@@ -2928,7 +2927,7 @@
         <v>59.17</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>43440.333340567129</v>
       </c>
@@ -2948,7 +2947,7 @@
         <v>72.17</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>43440.375007291666</v>
       </c>
@@ -2968,7 +2967,7 @@
         <v>77.48</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>43440.416674016204</v>
       </c>
@@ -2988,7 +2987,7 @@
         <v>67.08</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>43440.458340740741</v>
       </c>
@@ -3008,7 +3007,7 @@
         <v>60.81</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>43440.500007465278</v>
       </c>
@@ -3028,7 +3027,7 @@
         <v>57.15</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>43440.541674189815</v>
       </c>
@@ -3048,7 +3047,7 @@
         <v>65.73</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>43440.583340914352</v>
       </c>
@@ -3068,7 +3067,7 @@
         <v>58.89</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>43440.62500763889</v>
       </c>
@@ -3088,7 +3087,7 @@
         <v>60.7</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>43440.666674363427</v>
       </c>
@@ -3108,7 +3107,7 @@
         <v>78.430000000000007</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>43440.708341087964</v>
       </c>
@@ -3128,7 +3127,7 @@
         <v>93.64</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>43440.750007812501</v>
       </c>
@@ -3148,7 +3147,7 @@
         <v>86.34</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>43440.791674537038</v>
       </c>
@@ -3168,7 +3167,7 @@
         <v>85.72</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>43440.833341261576</v>
       </c>
@@ -3188,7 +3187,7 @@
         <v>76.12</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>43440.875007986113</v>
       </c>
@@ -3208,7 +3207,7 @@
         <v>61.78</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>43440.91667471065</v>
       </c>
@@ -3228,7 +3227,7 @@
         <v>61.55</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>43440.958341435187</v>
       </c>
@@ -3248,7 +3247,7 @@
         <v>63.49</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>43441.000008159725</v>
       </c>
@@ -3268,7 +3267,7 @@
         <v>58.07</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>43441.041674884262</v>
       </c>
@@ -3288,7 +3287,7 @@
         <v>52.05</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>43441.083341608799</v>
       </c>
@@ -3308,7 +3307,7 @@
         <v>53.69</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>43441.125008333336</v>
       </c>
@@ -3328,7 +3327,7 @@
         <v>50.57</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>43441.166675057873</v>
       </c>
@@ -3348,7 +3347,7 @@
         <v>56.83</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>43441.208341782411</v>
       </c>
@@ -3368,7 +3367,7 @@
         <v>56.54</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>43441.250008506948</v>
       </c>
@@ -3388,7 +3387,7 @@
         <v>59.97</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>43441.291675231485</v>
       </c>
@@ -3408,7 +3407,7 @@
         <v>83.78</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>43441.333341956015</v>
       </c>
@@ -3428,7 +3427,7 @@
         <v>70.22</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>43441.375008680552</v>
       </c>
@@ -3448,7 +3447,7 @@
         <v>88.41</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>43441.416675405089</v>
       </c>
@@ -3468,7 +3467,7 @@
         <v>75.459999999999994</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>43441.458342129627</v>
       </c>
@@ -3488,7 +3487,7 @@
         <v>69.55</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>43441.500008854164</v>
       </c>
@@ -3508,7 +3507,7 @@
         <v>78.55</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>43441.541675578701</v>
       </c>
@@ -3528,7 +3527,7 @@
         <v>79.73</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>43441.583342303238</v>
       </c>
@@ -3548,7 +3547,7 @@
         <v>140.31</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>43441.625009027775</v>
       </c>
@@ -3568,7 +3567,7 @@
         <v>55.15</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>43441.666675752313</v>
       </c>
@@ -3588,7 +3587,7 @@
         <v>66.41</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>43441.70834247685</v>
       </c>
@@ -3608,7 +3607,7 @@
         <v>65.349999999999994</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>43441.750009201387</v>
       </c>
@@ -3628,7 +3627,7 @@
         <v>116.82</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>43441.791675925924</v>
       </c>
@@ -3648,7 +3647,7 @@
         <v>75.14</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>43441.833342650461</v>
       </c>
@@ -3668,7 +3667,7 @@
         <v>70.260000000000005</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>43441.875009374999</v>
       </c>
@@ -3688,7 +3687,7 @@
         <v>60.22</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>43441.916676099536</v>
       </c>
@@ -3708,7 +3707,7 @@
         <v>57.25</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>43441.958342824073</v>
       </c>
@@ -3728,7 +3727,7 @@
         <v>73.08</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>43442.00000954861</v>
       </c>
@@ -3746,6 +3745,1446 @@
       </c>
       <c r="F169" s="1">
         <v>60.7</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A170" s="2">
+        <v>43442.041676273147</v>
+      </c>
+      <c r="B170" s="1">
+        <v>121.02</v>
+      </c>
+      <c r="C170" s="1">
+        <v>122.25</v>
+      </c>
+      <c r="D170" s="1">
+        <v>63.79</v>
+      </c>
+      <c r="E170" s="1">
+        <v>63.79</v>
+      </c>
+      <c r="F170" s="1">
+        <v>59.19</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A171" s="2">
+        <v>43442.083342997685</v>
+      </c>
+      <c r="B171" s="1">
+        <v>91.06</v>
+      </c>
+      <c r="C171" s="1">
+        <v>101.15</v>
+      </c>
+      <c r="D171" s="1">
+        <v>56.6</v>
+      </c>
+      <c r="E171" s="1">
+        <v>56.6</v>
+      </c>
+      <c r="F171" s="1">
+        <v>53.22</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A172" s="2">
+        <v>43442.125009722222</v>
+      </c>
+      <c r="B172" s="1">
+        <v>74.489999999999995</v>
+      </c>
+      <c r="C172" s="1">
+        <v>64.069999999999993</v>
+      </c>
+      <c r="D172" s="1">
+        <v>55.12</v>
+      </c>
+      <c r="E172" s="1">
+        <v>55.12</v>
+      </c>
+      <c r="F172" s="1">
+        <v>55.72</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173" s="2">
+        <v>43442.166676446759</v>
+      </c>
+      <c r="B173" s="1">
+        <v>64.69</v>
+      </c>
+      <c r="C173" s="1">
+        <v>67.92</v>
+      </c>
+      <c r="D173" s="1">
+        <v>58.36</v>
+      </c>
+      <c r="E173" s="1">
+        <v>58.36</v>
+      </c>
+      <c r="F173" s="1">
+        <v>59.1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174" s="2">
+        <v>43442.208343171296</v>
+      </c>
+      <c r="B174" s="1">
+        <v>72.73</v>
+      </c>
+      <c r="C174" s="1">
+        <v>69.239999999999995</v>
+      </c>
+      <c r="D174" s="1">
+        <v>60.45</v>
+      </c>
+      <c r="E174" s="1">
+        <v>60.45</v>
+      </c>
+      <c r="F174" s="1">
+        <v>56.59</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A175" s="2">
+        <v>43442.250009895834</v>
+      </c>
+      <c r="B175" s="1">
+        <v>87.37</v>
+      </c>
+      <c r="C175" s="1">
+        <v>88.18</v>
+      </c>
+      <c r="D175" s="1">
+        <v>58.45</v>
+      </c>
+      <c r="E175" s="1">
+        <v>58.45</v>
+      </c>
+      <c r="F175" s="1">
+        <v>50.21</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176" s="2">
+        <v>43442.291676620371</v>
+      </c>
+      <c r="B176" s="1">
+        <v>90.91</v>
+      </c>
+      <c r="C176" s="1">
+        <v>109.54</v>
+      </c>
+      <c r="D176" s="1">
+        <v>58.63</v>
+      </c>
+      <c r="E176" s="1">
+        <v>58.63</v>
+      </c>
+      <c r="F176" s="1">
+        <v>57.35</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177" s="2">
+        <v>43442.333343344908</v>
+      </c>
+      <c r="B177" s="1">
+        <v>120.77</v>
+      </c>
+      <c r="C177" s="1">
+        <v>133.78</v>
+      </c>
+      <c r="D177" s="1">
+        <v>62.42</v>
+      </c>
+      <c r="E177" s="1">
+        <v>62.42</v>
+      </c>
+      <c r="F177" s="1">
+        <v>63.38</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178" s="2">
+        <v>43442.375010069445</v>
+      </c>
+      <c r="B178" s="1">
+        <v>108.47</v>
+      </c>
+      <c r="C178" s="1">
+        <v>133.30000000000001</v>
+      </c>
+      <c r="D178" s="1">
+        <v>71.510000000000005</v>
+      </c>
+      <c r="E178" s="1">
+        <v>71.510000000000005</v>
+      </c>
+      <c r="F178" s="1">
+        <v>62.66</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179" s="2">
+        <v>43442.416676793982</v>
+      </c>
+      <c r="B179" s="1">
+        <v>115.27</v>
+      </c>
+      <c r="C179" s="1">
+        <v>126.27</v>
+      </c>
+      <c r="D179" s="1">
+        <v>64.8</v>
+      </c>
+      <c r="E179" s="1">
+        <v>64.8</v>
+      </c>
+      <c r="F179" s="1">
+        <v>60.87</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180" s="2">
+        <v>43442.45834351852</v>
+      </c>
+      <c r="B180" s="1">
+        <v>118.77</v>
+      </c>
+      <c r="C180" s="1">
+        <v>142.82</v>
+      </c>
+      <c r="D180" s="1">
+        <v>67.180000000000007</v>
+      </c>
+      <c r="E180" s="1">
+        <v>67.180000000000007</v>
+      </c>
+      <c r="F180" s="1">
+        <v>63.41</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181" s="2">
+        <v>43442.500010243057</v>
+      </c>
+      <c r="B181" s="1">
+        <v>165.14</v>
+      </c>
+      <c r="C181" s="1">
+        <v>269.27999999999997</v>
+      </c>
+      <c r="D181" s="1">
+        <v>72.989999999999995</v>
+      </c>
+      <c r="E181" s="1">
+        <v>72.989999999999995</v>
+      </c>
+      <c r="F181" s="1">
+        <v>64.84</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182" s="2">
+        <v>43442.541676967594</v>
+      </c>
+      <c r="B182" s="1">
+        <v>247.99</v>
+      </c>
+      <c r="C182" s="1">
+        <v>125.69</v>
+      </c>
+      <c r="D182" s="1">
+        <v>80.3</v>
+      </c>
+      <c r="E182" s="1">
+        <v>80.3</v>
+      </c>
+      <c r="F182" s="1">
+        <v>77.66</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183" s="2">
+        <v>43442.583343692131</v>
+      </c>
+      <c r="B183" s="1">
+        <v>103.96</v>
+      </c>
+      <c r="C183" s="1">
+        <v>128.75</v>
+      </c>
+      <c r="D183" s="1">
+        <v>90.18</v>
+      </c>
+      <c r="E183" s="1">
+        <v>90.18</v>
+      </c>
+      <c r="F183" s="1">
+        <v>73.400000000000006</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184" s="2">
+        <v>43442.625010416668</v>
+      </c>
+      <c r="B184" s="1">
+        <v>111.99</v>
+      </c>
+      <c r="C184" s="1">
+        <v>144.16</v>
+      </c>
+      <c r="D184" s="1">
+        <v>81.58</v>
+      </c>
+      <c r="E184" s="1">
+        <v>81.58</v>
+      </c>
+      <c r="F184" s="1">
+        <v>82.34</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185" s="2">
+        <v>43442.666677141206</v>
+      </c>
+      <c r="B185" s="1">
+        <v>86.02</v>
+      </c>
+      <c r="C185" s="1">
+        <v>88.7</v>
+      </c>
+      <c r="D185" s="1">
+        <v>88.09</v>
+      </c>
+      <c r="E185" s="1">
+        <v>88.09</v>
+      </c>
+      <c r="F185" s="1">
+        <v>75.16</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186" s="2">
+        <v>43442.708343865743</v>
+      </c>
+      <c r="B186" s="1">
+        <v>84.24</v>
+      </c>
+      <c r="C186" s="1">
+        <v>92.14</v>
+      </c>
+      <c r="D186" s="1">
+        <v>84.65</v>
+      </c>
+      <c r="E186" s="1">
+        <v>84.65</v>
+      </c>
+      <c r="F186" s="1">
+        <v>79.010000000000005</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187" s="2">
+        <v>43442.75001059028</v>
+      </c>
+      <c r="B187" s="1">
+        <v>87.97</v>
+      </c>
+      <c r="C187" s="1">
+        <v>102.01</v>
+      </c>
+      <c r="D187" s="1">
+        <v>85.62</v>
+      </c>
+      <c r="E187" s="1">
+        <v>85.62</v>
+      </c>
+      <c r="F187" s="1">
+        <v>84.02</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188" s="2">
+        <v>43442.791677314817</v>
+      </c>
+      <c r="B188" s="1">
+        <v>96.81</v>
+      </c>
+      <c r="C188" s="1">
+        <v>89.8</v>
+      </c>
+      <c r="D188" s="1">
+        <v>87.93</v>
+      </c>
+      <c r="E188" s="1">
+        <v>87.93</v>
+      </c>
+      <c r="F188" s="1">
+        <v>83.74</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189" s="2">
+        <v>43442.833344039354</v>
+      </c>
+      <c r="B189" s="1">
+        <v>81.88</v>
+      </c>
+      <c r="C189" s="1">
+        <v>87.23</v>
+      </c>
+      <c r="D189" s="1">
+        <v>79.95</v>
+      </c>
+      <c r="E189" s="1">
+        <v>79.95</v>
+      </c>
+      <c r="F189" s="1">
+        <v>82.15</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190" s="2">
+        <v>43442.875010763892</v>
+      </c>
+      <c r="B190" s="1">
+        <v>81.87</v>
+      </c>
+      <c r="C190" s="1">
+        <v>79.48</v>
+      </c>
+      <c r="D190" s="1">
+        <v>77.58</v>
+      </c>
+      <c r="E190" s="1">
+        <v>77.58</v>
+      </c>
+      <c r="F190" s="1">
+        <v>72.06</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191" s="2">
+        <v>43442.916677488429</v>
+      </c>
+      <c r="B191" s="1">
+        <v>76.97</v>
+      </c>
+      <c r="C191" s="1">
+        <v>68.27</v>
+      </c>
+      <c r="D191" s="1">
+        <v>73.33</v>
+      </c>
+      <c r="E191" s="1">
+        <v>73.33</v>
+      </c>
+      <c r="F191" s="1">
+        <v>62.87</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192" s="2">
+        <v>43442.958344212966</v>
+      </c>
+      <c r="B192" s="1">
+        <v>56.08</v>
+      </c>
+      <c r="C192" s="1">
+        <v>64.64</v>
+      </c>
+      <c r="D192" s="1">
+        <v>61.87</v>
+      </c>
+      <c r="E192" s="1">
+        <v>61.87</v>
+      </c>
+      <c r="F192" s="1">
+        <v>62.37</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193" s="2">
+        <v>43443.000010937503</v>
+      </c>
+      <c r="B193" s="1">
+        <v>63.69</v>
+      </c>
+      <c r="C193" s="1">
+        <v>74.06</v>
+      </c>
+      <c r="D193" s="1">
+        <v>60.03</v>
+      </c>
+      <c r="E193" s="1">
+        <v>60.03</v>
+      </c>
+      <c r="F193" s="1">
+        <v>58.56</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194" s="2">
+        <v>43443.04167766204</v>
+      </c>
+      <c r="B194" s="1">
+        <v>70.86</v>
+      </c>
+      <c r="C194" s="1">
+        <v>67.28</v>
+      </c>
+      <c r="D194" s="1">
+        <v>64.5</v>
+      </c>
+      <c r="E194" s="1">
+        <v>64.5</v>
+      </c>
+      <c r="F194" s="1">
+        <v>61.07</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195" s="2">
+        <v>43443.083344386578</v>
+      </c>
+      <c r="B195" s="1">
+        <v>68.62</v>
+      </c>
+      <c r="C195" s="1">
+        <v>57.07</v>
+      </c>
+      <c r="D195" s="1">
+        <v>63.39</v>
+      </c>
+      <c r="E195" s="1">
+        <v>63.39</v>
+      </c>
+      <c r="F195" s="1">
+        <v>55.32</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196" s="2">
+        <v>43443.125011111108</v>
+      </c>
+      <c r="B196" s="1">
+        <v>57.28</v>
+      </c>
+      <c r="C196" s="1">
+        <v>58.11</v>
+      </c>
+      <c r="D196" s="1">
+        <v>59.13</v>
+      </c>
+      <c r="E196" s="1">
+        <v>59.13</v>
+      </c>
+      <c r="F196" s="1">
+        <v>56.95</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197" s="2">
+        <v>43443.166677835645</v>
+      </c>
+      <c r="B197" s="1">
+        <v>55.73</v>
+      </c>
+      <c r="C197" s="1">
+        <v>57.48</v>
+      </c>
+      <c r="D197" s="1">
+        <v>59.64</v>
+      </c>
+      <c r="E197" s="1">
+        <v>59.64</v>
+      </c>
+      <c r="F197" s="1">
+        <v>56.91</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198" s="2">
+        <v>43443.208344560182</v>
+      </c>
+      <c r="B198" s="1">
+        <v>52.36</v>
+      </c>
+      <c r="C198" s="1">
+        <v>63.49</v>
+      </c>
+      <c r="D198" s="1">
+        <v>56.13</v>
+      </c>
+      <c r="E198" s="1">
+        <v>56.13</v>
+      </c>
+      <c r="F198" s="1">
+        <v>60.66</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A199" s="2">
+        <v>43443.250011284719</v>
+      </c>
+      <c r="B199" s="1">
+        <v>50.48</v>
+      </c>
+      <c r="C199" s="1">
+        <v>52.25</v>
+      </c>
+      <c r="D199" s="1">
+        <v>48.01</v>
+      </c>
+      <c r="E199" s="1">
+        <v>48.01</v>
+      </c>
+      <c r="F199" s="1">
+        <v>49.84</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A200" s="2">
+        <v>43443.291678009256</v>
+      </c>
+      <c r="B200" s="1">
+        <v>52.2</v>
+      </c>
+      <c r="C200" s="1">
+        <v>57.85</v>
+      </c>
+      <c r="D200" s="1">
+        <v>53.18</v>
+      </c>
+      <c r="E200" s="1">
+        <v>53.18</v>
+      </c>
+      <c r="F200" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A201" s="2">
+        <v>43443.333344733794</v>
+      </c>
+      <c r="B201" s="1">
+        <v>60.78</v>
+      </c>
+      <c r="C201" s="1">
+        <v>67.06</v>
+      </c>
+      <c r="D201" s="1">
+        <v>60.42</v>
+      </c>
+      <c r="E201" s="1">
+        <v>60.42</v>
+      </c>
+      <c r="F201" s="1">
+        <v>59.19</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A202" s="2">
+        <v>43443.375011458331</v>
+      </c>
+      <c r="B202" s="1">
+        <v>77.430000000000007</v>
+      </c>
+      <c r="C202" s="1">
+        <v>75.63</v>
+      </c>
+      <c r="D202" s="1">
+        <v>64.819999999999993</v>
+      </c>
+      <c r="E202" s="1">
+        <v>64.819999999999993</v>
+      </c>
+      <c r="F202" s="1">
+        <v>64.63</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A203" s="2">
+        <v>43443.416678182868</v>
+      </c>
+      <c r="B203" s="1">
+        <v>62.82</v>
+      </c>
+      <c r="C203" s="1">
+        <v>62.72</v>
+      </c>
+      <c r="D203" s="1">
+        <v>59.25</v>
+      </c>
+      <c r="E203" s="1">
+        <v>59.25</v>
+      </c>
+      <c r="F203" s="1">
+        <v>54.79</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A204" s="2">
+        <v>43443.458344907405</v>
+      </c>
+      <c r="B204" s="1">
+        <v>66.489999999999995</v>
+      </c>
+      <c r="C204" s="1">
+        <v>67.75</v>
+      </c>
+      <c r="D204" s="1">
+        <v>60.35</v>
+      </c>
+      <c r="E204" s="1">
+        <v>60.35</v>
+      </c>
+      <c r="F204" s="1">
+        <v>56.66</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A205" s="2">
+        <v>43443.500011631942</v>
+      </c>
+      <c r="B205" s="1">
+        <v>69.790000000000006</v>
+      </c>
+      <c r="C205" s="1">
+        <v>75.459999999999994</v>
+      </c>
+      <c r="D205" s="1">
+        <v>62.51</v>
+      </c>
+      <c r="E205" s="1">
+        <v>62.51</v>
+      </c>
+      <c r="F205" s="1">
+        <v>62.36</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A206" s="2">
+        <v>43443.54167835648</v>
+      </c>
+      <c r="B206" s="1">
+        <v>71.680000000000007</v>
+      </c>
+      <c r="C206" s="1">
+        <v>80.59</v>
+      </c>
+      <c r="D206" s="1">
+        <v>62.21</v>
+      </c>
+      <c r="E206" s="1">
+        <v>62.21</v>
+      </c>
+      <c r="F206" s="1">
+        <v>65.209999999999994</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207" s="2">
+        <v>43443.583345081017</v>
+      </c>
+      <c r="B207" s="1">
+        <v>79.94</v>
+      </c>
+      <c r="C207" s="1">
+        <v>77.040000000000006</v>
+      </c>
+      <c r="D207" s="1">
+        <v>72.569999999999993</v>
+      </c>
+      <c r="E207" s="1">
+        <v>72.569999999999993</v>
+      </c>
+      <c r="F207" s="1">
+        <v>66.33</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A208" s="2">
+        <v>43443.625011805554</v>
+      </c>
+      <c r="B208" s="1">
+        <v>78.260000000000005</v>
+      </c>
+      <c r="C208" s="1">
+        <v>82.22</v>
+      </c>
+      <c r="D208" s="1">
+        <v>80.23</v>
+      </c>
+      <c r="E208" s="1">
+        <v>80.23</v>
+      </c>
+      <c r="F208" s="1">
+        <v>71.06</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A209" s="2">
+        <v>43443.666678530091</v>
+      </c>
+      <c r="B209" s="1">
+        <v>83.6</v>
+      </c>
+      <c r="C209" s="1">
+        <v>90.24</v>
+      </c>
+      <c r="D209" s="1">
+        <v>86.23</v>
+      </c>
+      <c r="E209" s="1">
+        <v>86.23</v>
+      </c>
+      <c r="F209" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A210" s="2">
+        <v>43443.708345254629</v>
+      </c>
+      <c r="B210" s="1">
+        <v>82.98</v>
+      </c>
+      <c r="C210" s="1">
+        <v>113.86</v>
+      </c>
+      <c r="D210" s="1">
+        <v>87.06</v>
+      </c>
+      <c r="E210" s="1">
+        <v>87.06</v>
+      </c>
+      <c r="F210" s="1">
+        <v>98.81</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A211" s="2">
+        <v>43443.750011979166</v>
+      </c>
+      <c r="B211" s="1">
+        <v>108.7</v>
+      </c>
+      <c r="C211" s="1">
+        <v>105.07</v>
+      </c>
+      <c r="D211" s="1">
+        <v>113.08</v>
+      </c>
+      <c r="E211" s="1">
+        <v>113.08</v>
+      </c>
+      <c r="F211" s="1">
+        <v>96.45</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212" s="2">
+        <v>43443.791678703703</v>
+      </c>
+      <c r="B212" s="1">
+        <v>87.9</v>
+      </c>
+      <c r="C212" s="1">
+        <v>97.95</v>
+      </c>
+      <c r="D212" s="1">
+        <v>94.12</v>
+      </c>
+      <c r="E212" s="1">
+        <v>94.12</v>
+      </c>
+      <c r="F212" s="1">
+        <v>93.31</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A213" s="2">
+        <v>43443.83334542824</v>
+      </c>
+      <c r="B213" s="1">
+        <v>95.17</v>
+      </c>
+      <c r="C213" s="1">
+        <v>99.69</v>
+      </c>
+      <c r="D213" s="1">
+        <v>94.97</v>
+      </c>
+      <c r="E213" s="1">
+        <v>94.97</v>
+      </c>
+      <c r="F213" s="1">
+        <v>89.03</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A214" s="2">
+        <v>43443.875012152777</v>
+      </c>
+      <c r="B214" s="1">
+        <v>103.48</v>
+      </c>
+      <c r="C214" s="1">
+        <v>101.7</v>
+      </c>
+      <c r="D214" s="1">
+        <v>81.33</v>
+      </c>
+      <c r="E214" s="1">
+        <v>81.33</v>
+      </c>
+      <c r="F214" s="1">
+        <v>78.47</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A215" s="2">
+        <v>43443.916678877315</v>
+      </c>
+      <c r="B215" s="1">
+        <v>109.16</v>
+      </c>
+      <c r="C215" s="1">
+        <v>97.49</v>
+      </c>
+      <c r="D215" s="1">
+        <v>77.540000000000006</v>
+      </c>
+      <c r="E215" s="1">
+        <v>77.540000000000006</v>
+      </c>
+      <c r="F215" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A216" s="2">
+        <v>43443.958345601852</v>
+      </c>
+      <c r="B216" s="1">
+        <v>84.01</v>
+      </c>
+      <c r="C216" s="1">
+        <v>84.89</v>
+      </c>
+      <c r="D216" s="1">
+        <v>75.010000000000005</v>
+      </c>
+      <c r="E216" s="1">
+        <v>75.010000000000005</v>
+      </c>
+      <c r="F216" s="1">
+        <v>67.31</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A217" s="2">
+        <v>43444.000012326389</v>
+      </c>
+      <c r="B217" s="1">
+        <v>148.93</v>
+      </c>
+      <c r="C217" s="1">
+        <v>207.73</v>
+      </c>
+      <c r="D217" s="1">
+        <v>64</v>
+      </c>
+      <c r="E217" s="1">
+        <v>64</v>
+      </c>
+      <c r="F217" s="1">
+        <v>62.54</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A218" s="2">
+        <v>43444.041679050926</v>
+      </c>
+      <c r="B218" s="1">
+        <v>104.11</v>
+      </c>
+      <c r="C218" s="1">
+        <v>75.97</v>
+      </c>
+      <c r="D218" s="1">
+        <v>73.25</v>
+      </c>
+      <c r="E218" s="1">
+        <v>73.25</v>
+      </c>
+      <c r="F218" s="1">
+        <v>61.75</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A219" s="2">
+        <v>43444.083345775463</v>
+      </c>
+      <c r="B219" s="1">
+        <v>81.36</v>
+      </c>
+      <c r="C219" s="1">
+        <v>56.49</v>
+      </c>
+      <c r="D219" s="1">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="E219" s="1">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="F219" s="1">
+        <v>50.56</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A220" s="2">
+        <v>43444.125012500001</v>
+      </c>
+      <c r="B220" s="1">
+        <v>47.13</v>
+      </c>
+      <c r="C220" s="1">
+        <v>51.52</v>
+      </c>
+      <c r="D220" s="1">
+        <v>52.73</v>
+      </c>
+      <c r="E220" s="1">
+        <v>52.73</v>
+      </c>
+      <c r="F220" s="1">
+        <v>49.34</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221" s="2">
+        <v>43444.166679224538</v>
+      </c>
+      <c r="B221" s="1">
+        <v>45.25</v>
+      </c>
+      <c r="C221" s="1">
+        <v>52.68</v>
+      </c>
+      <c r="D221" s="1">
+        <v>52.21</v>
+      </c>
+      <c r="E221" s="1">
+        <v>52.21</v>
+      </c>
+      <c r="F221" s="1">
+        <v>51.16</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222" s="2">
+        <v>43444.208345949075</v>
+      </c>
+      <c r="B222" s="1">
+        <v>57.41</v>
+      </c>
+      <c r="C222" s="1">
+        <v>59.65</v>
+      </c>
+      <c r="D222" s="1">
+        <v>67.27</v>
+      </c>
+      <c r="E222" s="1">
+        <v>67.27</v>
+      </c>
+      <c r="F222" s="1">
+        <v>54.53</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A223" s="2">
+        <v>43444.250012673612</v>
+      </c>
+      <c r="B223" s="1">
+        <v>62.8</v>
+      </c>
+      <c r="C223" s="1">
+        <v>86.33</v>
+      </c>
+      <c r="D223" s="1">
+        <v>65.66</v>
+      </c>
+      <c r="E223" s="1">
+        <v>65.66</v>
+      </c>
+      <c r="F223" s="1">
+        <v>63.93</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A224" s="2">
+        <v>43444.291679398149</v>
+      </c>
+      <c r="B224" s="1">
+        <v>82.91</v>
+      </c>
+      <c r="C224" s="1">
+        <v>116.57</v>
+      </c>
+      <c r="D224" s="1">
+        <v>83.1</v>
+      </c>
+      <c r="E224" s="1">
+        <v>83.1</v>
+      </c>
+      <c r="F224" s="1">
+        <v>88.65</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A225" s="2">
+        <v>43444.333346122687</v>
+      </c>
+      <c r="B225" s="1">
+        <v>96.97</v>
+      </c>
+      <c r="C225" s="1">
+        <v>94.64</v>
+      </c>
+      <c r="D225" s="1">
+        <v>99.48</v>
+      </c>
+      <c r="E225" s="1">
+        <v>99.48</v>
+      </c>
+      <c r="F225" s="1">
+        <v>80.540000000000006</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A226" s="2">
+        <v>43444.375012847224</v>
+      </c>
+      <c r="B226" s="1">
+        <v>82.99</v>
+      </c>
+      <c r="C226" s="1">
+        <v>93.04</v>
+      </c>
+      <c r="D226" s="1">
+        <v>89.06</v>
+      </c>
+      <c r="E226" s="1">
+        <v>89.06</v>
+      </c>
+      <c r="F226" s="1">
+        <v>80.13</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A227" s="2">
+        <v>43444.416679571761</v>
+      </c>
+      <c r="B227" s="1">
+        <v>83.22</v>
+      </c>
+      <c r="C227" s="1">
+        <v>102.57</v>
+      </c>
+      <c r="D227" s="1">
+        <v>89.88</v>
+      </c>
+      <c r="E227" s="1">
+        <v>89.88</v>
+      </c>
+      <c r="F227" s="1">
+        <v>84.42</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A228" s="2">
+        <v>43444.458346296298</v>
+      </c>
+      <c r="B228" s="1">
+        <v>83.12</v>
+      </c>
+      <c r="C228" s="1">
+        <v>86.49</v>
+      </c>
+      <c r="D228" s="1">
+        <v>94.11</v>
+      </c>
+      <c r="E228" s="1">
+        <v>94.11</v>
+      </c>
+      <c r="F228" s="1">
+        <v>71.55</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A229" s="2">
+        <v>43444.500013020835</v>
+      </c>
+      <c r="B229" s="1">
+        <v>80.92</v>
+      </c>
+      <c r="C229" s="1">
+        <v>94.6</v>
+      </c>
+      <c r="D229" s="1">
+        <v>86.52</v>
+      </c>
+      <c r="E229" s="1">
+        <v>86.52</v>
+      </c>
+      <c r="F229" s="1">
+        <v>81.69</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A230" s="2">
+        <v>43444.541679745373</v>
+      </c>
+      <c r="B230" s="1">
+        <v>86.26</v>
+      </c>
+      <c r="C230" s="1">
+        <v>96.31</v>
+      </c>
+      <c r="D230" s="1">
+        <v>92.69</v>
+      </c>
+      <c r="E230" s="1">
+        <v>92.69</v>
+      </c>
+      <c r="F230" s="1">
+        <v>84.33</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A231" s="2">
+        <v>43444.58334646991</v>
+      </c>
+      <c r="B231" s="1">
+        <v>130.55000000000001</v>
+      </c>
+      <c r="C231" s="1">
+        <v>90.91</v>
+      </c>
+      <c r="D231" s="1">
+        <v>140.16999999999999</v>
+      </c>
+      <c r="E231" s="1">
+        <v>140.16999999999999</v>
+      </c>
+      <c r="F231" s="1">
+        <v>80.650000000000006</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A232" s="2">
+        <v>43444.625013194447</v>
+      </c>
+      <c r="B232" s="1">
+        <v>88.69</v>
+      </c>
+      <c r="C232" s="1">
+        <v>100.1</v>
+      </c>
+      <c r="D232" s="1">
+        <v>99.02</v>
+      </c>
+      <c r="E232" s="1">
+        <v>99.02</v>
+      </c>
+      <c r="F232" s="1">
+        <v>91.55</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A233" s="2">
+        <v>43444.666679918984</v>
+      </c>
+      <c r="B233" s="1">
+        <v>86.6</v>
+      </c>
+      <c r="C233" s="1">
+        <v>141.06</v>
+      </c>
+      <c r="D233" s="1">
+        <v>99.61</v>
+      </c>
+      <c r="E233" s="1">
+        <v>99.61</v>
+      </c>
+      <c r="F233" s="1">
+        <v>149.1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A234" s="2">
+        <v>43444.708346643522</v>
+      </c>
+      <c r="B234" s="1">
+        <v>83.45</v>
+      </c>
+      <c r="C234" s="1">
+        <v>104.08</v>
+      </c>
+      <c r="D234" s="1">
+        <v>91.88</v>
+      </c>
+      <c r="E234" s="1">
+        <v>91.88</v>
+      </c>
+      <c r="F234" s="1">
+        <v>105.15</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A235" s="2">
+        <v>43444.750013368059</v>
+      </c>
+      <c r="B235" s="1">
+        <v>85.99</v>
+      </c>
+      <c r="C235" s="1">
+        <v>97.42</v>
+      </c>
+      <c r="D235" s="1">
+        <v>97.04</v>
+      </c>
+      <c r="E235" s="1">
+        <v>97.04</v>
+      </c>
+      <c r="F235" s="1">
+        <v>94.67</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A236" s="2">
+        <v>43444.791680092596</v>
+      </c>
+      <c r="B236" s="1">
+        <v>84.52</v>
+      </c>
+      <c r="C236" s="1">
+        <v>98.31</v>
+      </c>
+      <c r="D236" s="1">
+        <v>89.12</v>
+      </c>
+      <c r="E236" s="1">
+        <v>89.12</v>
+      </c>
+      <c r="F236" s="1">
+        <v>99.64</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A237" s="2">
+        <v>43444.833346817133</v>
+      </c>
+      <c r="B237" s="1">
+        <v>85.23</v>
+      </c>
+      <c r="C237" s="1">
+        <v>99.06</v>
+      </c>
+      <c r="D237" s="1">
+        <v>99.66</v>
+      </c>
+      <c r="E237" s="1">
+        <v>99.66</v>
+      </c>
+      <c r="F237" s="1">
+        <v>100.75</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A238" s="2">
+        <v>43444.875013541663</v>
+      </c>
+      <c r="B238" s="1">
+        <v>95.46</v>
+      </c>
+      <c r="C238" s="1">
+        <v>96.84</v>
+      </c>
+      <c r="D238" s="1">
+        <v>99.28</v>
+      </c>
+      <c r="E238" s="1">
+        <v>99.28</v>
+      </c>
+      <c r="F238" s="1">
+        <v>80.37</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A239" s="2">
+        <v>43444.9166802662</v>
+      </c>
+      <c r="B239" s="1">
+        <v>79.010000000000005</v>
+      </c>
+      <c r="C239" s="1">
+        <v>104.64</v>
+      </c>
+      <c r="D239" s="1">
+        <v>74.59</v>
+      </c>
+      <c r="E239" s="1">
+        <v>74.59</v>
+      </c>
+      <c r="F239" s="1">
+        <v>63.16</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A240" s="2">
+        <v>43444.958346990737</v>
+      </c>
+      <c r="B240" s="1">
+        <v>79.239999999999995</v>
+      </c>
+      <c r="C240" s="1">
+        <v>81.069999999999993</v>
+      </c>
+      <c r="D240" s="1">
+        <v>83.06</v>
+      </c>
+      <c r="E240" s="1">
+        <v>83.06</v>
+      </c>
+      <c r="F240" s="1">
+        <v>75.27</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A241" s="2">
+        <v>43445.000013715275</v>
+      </c>
+      <c r="B241" s="1">
+        <v>83.12</v>
+      </c>
+      <c r="C241" s="1">
+        <v>103.88</v>
+      </c>
+      <c r="D241" s="1">
+        <v>72.58</v>
+      </c>
+      <c r="E241" s="1">
+        <v>72.58</v>
+      </c>
+      <c r="F241" s="1">
+        <v>66.760000000000005</v>
       </c>
     </row>
   </sheetData>
@@ -3755,733 +5194,733 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A241"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" s="1"/>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" s="1"/>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" s="1"/>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" s="1"/>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" s="1"/>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" s="1"/>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" s="1"/>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" s="1"/>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" s="1"/>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" s="1"/>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" s="1"/>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" s="1"/>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" s="1"/>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" s="1"/>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" s="1"/>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" s="1"/>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" s="1"/>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" s="1"/>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" s="1"/>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" s="1"/>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" s="1"/>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" s="1"/>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" s="1"/>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225" s="1"/>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" s="1"/>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227" s="1"/>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" s="1"/>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" s="1"/>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" s="1"/>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" s="1"/>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" s="1"/>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" s="1"/>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234" s="1"/>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" s="1"/>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" s="1"/>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" s="1"/>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" s="1"/>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239" s="1"/>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" s="1"/>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241" s="1"/>
     </row>
   </sheetData>

</xml_diff>